<commit_message>
Loot HUD and bug fix
</commit_message>
<xml_diff>
--- a/Excel/Loot.xlsx
+++ b/Excel/Loot.xlsx
@@ -8,24 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Unity\Steam Multiplayer Template\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D767DF00-0902-47F9-B7B6-5F16C43A8E4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CBD8026-B1CB-4075-94ED-E972D7256002}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="50">
   <si>
     <t>id</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -171,19 +182,7 @@
     <t>16</t>
   </si>
   <si>
-    <t>16</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>8</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>空</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>32</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -225,6 +224,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="0.00_);[Red]\(0.00\)"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -283,7 +285,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -292,6 +294,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -574,7 +582,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:A2"/>
@@ -589,304 +597,307 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="4">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="3" t="s">
+      <c r="C19" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="3" t="s">
+      <c r="C20" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="D22" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D23" s="5"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B14:B17">

</xml_diff>